<commit_message>
update scrittura file .sfr per diversi stress period; non funziona
</commit_message>
<xml_diff>
--- a/MAURICE/test_models/m19_sfr_data.xlsx
+++ b/MAURICE/test_models/m19_sfr_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\hm\MAURICE\test_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09941BAF-F354-4578-94D9-09E7E2172676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46180913-0C13-4C48-8F57-3CD4D5408F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{3815B33F-C467-47DB-BE3E-F164846AD30F}"/>
+    <workbookView xWindow="-40" yWindow="-40" windowWidth="19280" windowHeight="10160" xr2:uid="{3815B33F-C467-47DB-BE3E-F164846AD30F}"/>
   </bookViews>
   <sheets>
     <sheet name="ITEM1" sheetId="2" r:id="rId1"/>
@@ -88,15 +88,6 @@
   </si>
   <si>
     <t>ISFROPT</t>
-  </si>
-  <si>
-    <t>NOTSURE1</t>
-  </si>
-  <si>
-    <t>NOTSURE2</t>
-  </si>
-  <si>
-    <t>NOTSURE3</t>
   </si>
   <si>
     <t>ITMP</t>
@@ -184,6 +175,15 @@
   </si>
   <si>
     <t>z</t>
+  </si>
+  <si>
+    <t>NSTRAIL</t>
+  </si>
+  <si>
+    <t>ISUZN</t>
+  </si>
+  <si>
+    <t>NSFRSETS</t>
   </si>
 </sst>
 </file>
@@ -561,11 +561,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5CC6E6-61D0-4A7E-8B48-533D5D72D4B4}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
@@ -596,18 +599,18 @@
         <v>15</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="K1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="L1" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A2">
-        <v>-174</v>
+        <v>-173</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -625,7 +628,7 @@
         <v>1E-4</v>
       </c>
       <c r="G2">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H2">
         <v>54</v>
@@ -660,7 +663,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -5199,16 +5202,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.75">
@@ -5234,8 +5237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F66ED0-3422-4DE9-BF71-3028C78BAFA0}">
   <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -5245,40 +5248,40 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" t="s">
-        <v>31</v>
-      </c>
       <c r="L1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.75">
@@ -5697,34 +5700,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>42</v>
-      </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.75">
@@ -5732,7 +5735,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -5771,7 +5774,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2">
         <v>3.29</v>
@@ -5803,7 +5806,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -5842,7 +5845,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2">
         <v>3.29</v>
@@ -5874,7 +5877,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -5913,7 +5916,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C7" s="2">
         <v>3.29</v>
@@ -5945,7 +5948,7 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -5984,7 +5987,7 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2">
         <v>3.29</v>
@@ -6016,7 +6019,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2">
         <v>0</v>
@@ -6055,7 +6058,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="2">
         <v>3.29</v>
@@ -6087,7 +6090,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -6126,7 +6129,7 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C13" s="2">
         <v>3.29</v>
@@ -6158,7 +6161,7 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14" s="2">
         <v>0</v>
@@ -6197,7 +6200,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" s="2">
         <v>3.29</v>

</xml_diff>